<commit_message>
remove # in front of plate number
</commit_message>
<xml_diff>
--- a/inst/extdata/Plate_design_example.xlsx
+++ b/inst/extdata/Plate_design_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\glycodash\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vf-lumc-home.lumcnet.prod.intern\lumc-home$\sgijze\MyDocs\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61B776B-6E80-4AC7-8A63-30249C1F1859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C30AD90-43CB-4BCA-8C80-39F1162631A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="18675" windowHeight="10005" xr2:uid="{640FE4C3-9150-49CA-984F-C3B2E4C26F7E}"/>
+    <workbookView xWindow="22714" yWindow="-231" windowWidth="23040" windowHeight="13897" xr2:uid="{640FE4C3-9150-49CA-984F-C3B2E4C26F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="19">
   <si>
-    <t>Plate #1</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -74,25 +71,28 @@
     <t>H</t>
   </si>
   <si>
-    <t>Plate #2</t>
-  </si>
-  <si>
-    <t>Plate #3</t>
-  </si>
-  <si>
     <t>IVIGg</t>
   </si>
   <si>
-    <t>Plate #4</t>
-  </si>
-  <si>
-    <t>Plate #5</t>
-  </si>
-  <si>
-    <t>Plate #6</t>
-  </si>
-  <si>
-    <t>Plate #7</t>
+    <t>Plate 1</t>
+  </si>
+  <si>
+    <t>Plate 2</t>
+  </si>
+  <si>
+    <t>Plate 3</t>
+  </si>
+  <si>
+    <t>Plate 4</t>
+  </si>
+  <si>
+    <t>Plate 5</t>
+  </si>
+  <si>
+    <t>Plate 6</t>
+  </si>
+  <si>
+    <t>Plate 7</t>
   </si>
 </sst>
 </file>
@@ -446,18 +446,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7E8C05-E64E-41C6-BE60-5D221617EAD1}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -498,71 +498,71 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -603,71 +603,71 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -708,69 +708,69 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -816,69 +816,69 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -924,69 +924,69 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -1032,69 +1032,69 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L52" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I53" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -1140,69 +1140,69 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J63" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G68" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1216,7 +1216,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1228,7 +1228,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fixes. Calculate custom derived traits for multiple clusters
</commit_message>
<xml_diff>
--- a/inst/extdata/Plate_design_example.xlsx
+++ b/inst/extdata/Plate_design_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vf-lumc-home.lumcnet.prod.intern\lumc-home$\sgijze\MyDocs\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C30AD90-43CB-4BCA-8C80-39F1162631A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78EB70F-DEC5-4474-839A-5028C29B58C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22714" yWindow="-231" windowWidth="23040" windowHeight="13897" xr2:uid="{640FE4C3-9150-49CA-984F-C3B2E4C26F7E}"/>
   </bookViews>
@@ -446,9 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7E8C05-E64E-41C6-BE60-5D221617EAD1}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>